<commit_message>
ajuste no cálculo para remover anos sem dado sobre o efetivo do rebanho
</commit_message>
<xml_diff>
--- a/Data/g3.5a.xlsx
+++ b/Data/g3.5a.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="g3.5a 2025" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="g3.5a 2023" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9.745504422214712</v>
+        <v>32.069953084778</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -466,11 +466,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Mato Grosso do Sul</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.439113564332414</v>
+        <v>17.53196975891699</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
@@ -479,11 +479,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mato Grosso do Sul</t>
+          <t>Mato Grosso</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5.069771642008148</v>
+        <v>17.49915955766788</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
@@ -492,11 +492,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Mato Grosso</t>
+          <t>Sergipe</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.905188573843787</v>
+        <v>17.46029783768665</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.664015655880712</v>
+        <v>15.89086868026616</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
@@ -518,11 +518,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Pernambuco</t>
+          <t>Goiás</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.439924387665076</v>
+        <v>14.91689084958633</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4.135806961409583</v>
+        <v>14.29087477237749</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2.405111618563228</v>
+        <v>8.045879236039708</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
g3.5 - correção do nome da aba e inclusão do ano na planilha
</commit_message>
<xml_diff>
--- a/Data/g3.5a.xlsx
+++ b/Data/g3.5a.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="g3.5a 2023" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="g3.5a" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>Ordem</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ano</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -462,6 +467,9 @@
       <c r="C2" t="n">
         <v>1</v>
       </c>
+      <c r="D2" t="n">
+        <v>2023</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -475,6 +483,9 @@
       <c r="C3" t="n">
         <v>2</v>
       </c>
+      <c r="D3" t="n">
+        <v>2023</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -488,6 +499,9 @@
       <c r="C4" t="n">
         <v>3</v>
       </c>
+      <c r="D4" t="n">
+        <v>2023</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -501,6 +515,9 @@
       <c r="C5" t="n">
         <v>4</v>
       </c>
+      <c r="D5" t="n">
+        <v>2023</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -514,6 +531,9 @@
       <c r="C6" t="n">
         <v>5</v>
       </c>
+      <c r="D6" t="n">
+        <v>2023</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -527,6 +547,9 @@
       <c r="C7" t="n">
         <v>6</v>
       </c>
+      <c r="D7" t="n">
+        <v>2023</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -538,6 +561,9 @@
         <v>14.29087477237749</v>
       </c>
       <c r="C8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>2023</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -549,6 +575,9 @@
         <v>8.045879236039708</v>
       </c>
       <c r="C9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>2023</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>